<commit_message>
updated documentation so can be updated athome
</commit_message>
<xml_diff>
--- a/Graph Results/Graph Results.xlsx
+++ b/Graph Results/Graph Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" tabRatio="641" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Facebook" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="63">
   <si>
     <t>Edges</t>
   </si>
@@ -205,6 +205,21 @@
   </si>
   <si>
     <t>*Note: the spanning trees are rooted by a vertex with median degree.  The results for this graph are that the roots create insignificant trees</t>
+  </si>
+  <si>
+    <t>Tree 3 v2</t>
+  </si>
+  <si>
+    <t>Approx. Diameter (14)</t>
+  </si>
+  <si>
+    <t>Tree 5 v2</t>
+  </si>
+  <si>
+    <t>Tree 3v2</t>
+  </si>
+  <si>
+    <t>Tree 3 v5</t>
   </si>
 </sst>
 </file>
@@ -538,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17:Q20"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +569,7 @@
     <col min="17" max="17" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
@@ -603,8 +618,14 @@
       <c r="Q1" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -656,8 +677,14 @@
       <c r="Q2">
         <v>41284</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>4988</v>
+      </c>
+      <c r="S2">
+        <v>5942</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -709,8 +736,14 @@
       <c r="Q3">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>8</v>
+      </c>
+      <c r="S3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -762,8 +795,14 @@
       <c r="Q4">
         <v>4039</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>4039</v>
+      </c>
+      <c r="S4">
+        <v>4039</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -815,13 +854,14 @@
       <c r="Q5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -870,8 +910,14 @@
       <c r="Q7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>1000</v>
+      </c>
+      <c r="S7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -920,8 +966,14 @@
       <c r="Q8">
         <v>668</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>940</v>
+      </c>
+      <c r="S8">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -970,8 +1022,14 @@
       <c r="Q9">
         <v>285</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>56</v>
+      </c>
+      <c r="S9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1020,8 +1078,14 @@
       <c r="Q10">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>4</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1070,8 +1134,14 @@
       <c r="Q11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1120,8 +1190,14 @@
       <c r="Q12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1170,8 +1246,14 @@
       <c r="Q13">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1211,8 +1293,14 @@
       <c r="Q15">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>11</v>
+      </c>
+      <c r="S15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1251,6 +1339,12 @@
       </c>
       <c r="Q16">
         <v>1</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -1318,7 +1412,7 @@
         <v>13</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="2"/>
+        <f>SUM(Q15, Q16)</f>
         <v>14</v>
       </c>
     </row>
@@ -1536,10 +1630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1548,7 +1642,7 @@
     <col min="13" max="13" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
@@ -1585,8 +1679,14 @@
       <c r="M1" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1626,8 +1726,14 @@
       <c r="M2">
         <v>12908</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>9685</v>
+      </c>
+      <c r="O2">
+        <v>10728</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1667,8 +1773,14 @@
       <c r="M3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>10</v>
+      </c>
+      <c r="O3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -1708,8 +1820,14 @@
       <c r="M4">
         <v>6474</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>6474</v>
+      </c>
+      <c r="O4">
+        <v>6474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1749,13 +1867,19 @@
       <c r="M5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1792,8 +1916,14 @@
       <c r="M7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>1000</v>
+      </c>
+      <c r="O7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1830,8 +1960,14 @@
       <c r="M8">
         <v>730</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>830</v>
+      </c>
+      <c r="O8">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1868,8 +2004,14 @@
       <c r="M9">
         <v>252</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>161</v>
+      </c>
+      <c r="O9">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1906,8 +2048,14 @@
       <c r="M10">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>9</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1944,8 +2092,14 @@
       <c r="M11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1982,8 +2136,14 @@
       <c r="M12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2020,8 +2180,14 @@
       <c r="M13">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2058,8 +2224,14 @@
       <c r="M15">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>14</v>
+      </c>
+      <c r="O15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -2095,6 +2267,12 @@
       </c>
       <c r="M16">
         <v>0</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -2303,10 +2481,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2319,7 +2497,7 @@
     <col min="17" max="17" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2368,8 +2546,14 @@
       <c r="Q1" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2421,8 +2605,14 @@
       <c r="Q2">
         <v>69213</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>37107</v>
+      </c>
+      <c r="S2">
+        <v>42761</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2468,8 +2658,14 @@
       <c r="Q3">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>15</v>
+      </c>
+      <c r="S3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -2515,8 +2711,14 @@
       <c r="Q4">
         <v>21363</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>21363</v>
+      </c>
+      <c r="S4">
+        <v>21363</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2562,13 +2764,19 @@
       <c r="Q5">
         <v>85734</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>86938</v>
+      </c>
+      <c r="S5">
+        <v>86938</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2611,8 +2819,14 @@
       <c r="Q7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>100</v>
+      </c>
+      <c r="S7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -2655,8 +2869,14 @@
       <c r="Q8">
         <v>978</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>975</v>
+      </c>
+      <c r="S8">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -2699,8 +2919,14 @@
       <c r="Q9">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>20</v>
+      </c>
+      <c r="S9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -2743,8 +2969,14 @@
       <c r="Q10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>4</v>
+      </c>
+      <c r="S10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2787,8 +3019,14 @@
       <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -2831,8 +3069,14 @@
       <c r="Q12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -2875,8 +3119,14 @@
       <c r="Q13">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -2907,8 +3157,14 @@
       <c r="Q15">
         <v>150</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>106</v>
+      </c>
+      <c r="S15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -2938,6 +3194,12 @@
       </c>
       <c r="Q16">
         <v>13</v>
+      </c>
+      <c r="R16">
+        <v>49</v>
+      </c>
+      <c r="S16">
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -2949,7 +3211,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:N17" si="0">SUM(C15, C16)</f>
+        <f t="shared" ref="C17:M17" si="0">SUM(C15, C16)</f>
         <v>0</v>
       </c>
       <c r="D17">
@@ -3018,7 +3280,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" ref="C18:N18" si="5">C15/163</f>
+        <f t="shared" ref="C18:M18" si="5">C15/163</f>
         <v>0</v>
       </c>
       <c r="D18" s="2">
@@ -3083,7 +3345,7 @@
         <v>48</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" ref="B19:N20" si="7">B16/163</f>
+        <f t="shared" ref="B19:M20" si="7">B16/163</f>
         <v>0</v>
       </c>
       <c r="C19" s="2">
@@ -3228,10 +3490,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3244,7 +3506,7 @@
     <col min="17" max="17" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3293,8 +3555,14 @@
       <c r="Q1" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -3346,10 +3614,16 @@
       <c r="Q2">
         <v>104885</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>36660</v>
+      </c>
+      <c r="S2">
+        <v>46036</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="B3">
         <v>13</v>
@@ -3393,8 +3667,14 @@
       <c r="Q3">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>13</v>
+      </c>
+      <c r="S3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -3440,8 +3720,14 @@
       <c r="Q4">
         <v>17903</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>17903</v>
+      </c>
+      <c r="S4">
+        <v>17903</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -3487,13 +3773,19 @@
       <c r="Q5">
         <v>114798</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>115378</v>
+      </c>
+      <c r="S5">
+        <v>115378</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -3536,8 +3828,14 @@
       <c r="Q7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>1000</v>
+      </c>
+      <c r="S7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -3580,8 +3878,14 @@
       <c r="Q8">
         <v>987</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>989</v>
+      </c>
+      <c r="S8">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3624,8 +3928,14 @@
       <c r="Q9">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>6</v>
+      </c>
+      <c r="S9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -3668,8 +3978,14 @@
       <c r="Q10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>5</v>
+      </c>
+      <c r="S10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -3712,8 +4028,14 @@
       <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -3756,8 +4078,14 @@
       <c r="Q12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3800,8 +4128,14 @@
       <c r="Q13">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -3832,8 +4166,14 @@
       <c r="Q15">
         <v>174</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>70</v>
+      </c>
+      <c r="S15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -3863,6 +4203,12 @@
       </c>
       <c r="Q16">
         <v>26</v>
+      </c>
+      <c r="R16">
+        <v>91</v>
+      </c>
+      <c r="S16">
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -4153,10 +4499,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17:Q20"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4168,7 +4514,7 @@
     <col min="17" max="17" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
@@ -4217,8 +4563,14 @@
       <c r="Q1" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -4270,8 +4622,14 @@
       <c r="Q2">
         <v>121755</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>52497</v>
+      </c>
+      <c r="S2">
+        <v>64422</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -4323,8 +4681,14 @@
       <c r="Q3">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>14</v>
+      </c>
+      <c r="S3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -4376,8 +4740,14 @@
       <c r="Q4">
         <v>33696</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>33696</v>
+      </c>
+      <c r="S4">
+        <v>33696</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -4429,13 +4799,19 @@
       <c r="Q5">
         <v>1065</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>2997</v>
+      </c>
+      <c r="S5">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4484,8 +4860,14 @@
       <c r="Q7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>1000</v>
+      </c>
+      <c r="S7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -4534,8 +4916,14 @@
       <c r="Q8">
         <v>745</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>443</v>
+      </c>
+      <c r="S8">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4584,8 +4972,14 @@
       <c r="Q9">
         <v>251</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>453</v>
+      </c>
+      <c r="S9">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -4634,8 +5028,14 @@
       <c r="Q10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>101</v>
+      </c>
+      <c r="S10">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -4684,8 +5084,14 @@
       <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>3</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -4734,8 +5140,14 @@
       <c r="Q12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -4784,8 +5196,14 @@
       <c r="Q13">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -4822,8 +5240,14 @@
       <c r="Q15">
         <v>55</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>48</v>
+      </c>
+      <c r="S15">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -4859,6 +5283,12 @@
       </c>
       <c r="Q16">
         <v>1</v>
+      </c>
+      <c r="R16">
+        <v>8</v>
+      </c>
+      <c r="S16">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -5144,10 +5574,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17:Q20"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5160,7 +5590,7 @@
     <col min="17" max="17" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
@@ -5209,8 +5639,14 @@
       <c r="Q1" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -5262,8 +5698,14 @@
       <c r="Q2">
         <v>244735</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>112636</v>
+      </c>
+      <c r="S2">
+        <v>135776</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -5315,8 +5757,14 @@
       <c r="Q3">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>11</v>
+      </c>
+      <c r="S3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -5368,8 +5816,14 @@
       <c r="Q4">
         <v>75877</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>75877</v>
+      </c>
+      <c r="S4">
+        <v>75877</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -5421,13 +5875,19 @@
       <c r="Q5">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>12</v>
+      </c>
+      <c r="S5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -5476,8 +5936,14 @@
       <c r="Q7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>1000</v>
+      </c>
+      <c r="S7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -5526,8 +5992,14 @@
       <c r="Q8">
         <v>750</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>463</v>
+      </c>
+      <c r="S8">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -5576,8 +6048,14 @@
       <c r="Q9">
         <v>247</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>483</v>
+      </c>
+      <c r="S9">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -5626,8 +6104,14 @@
       <c r="Q10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>52</v>
+      </c>
+      <c r="S10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -5676,8 +6160,14 @@
       <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>2</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -5726,8 +6216,14 @@
       <c r="Q12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -5776,8 +6272,14 @@
       <c r="Q13">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -5814,8 +6316,14 @@
       <c r="Q15">
         <v>110</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>105</v>
+      </c>
+      <c r="S15">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -5851,6 +6359,12 @@
       </c>
       <c r="Q16">
         <v>4</v>
+      </c>
+      <c r="R16">
+        <v>9</v>
+      </c>
+      <c r="S16">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -6137,10 +6651,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S17" sqref="S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6153,7 +6667,7 @@
     <col min="17" max="17" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
@@ -6202,8 +6716,14 @@
       <c r="Q1" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6255,8 +6775,14 @@
       <c r="Q2">
         <v>2280120</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>1492114</v>
+      </c>
+      <c r="S2">
+        <v>1689731</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -6305,8 +6831,14 @@
       <c r="Q3">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>16</v>
+      </c>
+      <c r="S3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -6355,8 +6887,14 @@
       <c r="Q4">
         <v>1134890</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>1134890</v>
+      </c>
+      <c r="S4">
+        <v>1134890</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -6405,13 +6943,19 @@
       <c r="Q5">
         <v>22939</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>22939</v>
+      </c>
+      <c r="S5">
+        <v>22939</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -6454,8 +6998,14 @@
       <c r="Q7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>1000</v>
+      </c>
+      <c r="S7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -6498,8 +7048,14 @@
       <c r="Q8">
         <v>698</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>703</v>
+      </c>
+      <c r="S8">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -6542,8 +7098,14 @@
       <c r="Q9">
         <v>302</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>279</v>
+      </c>
+      <c r="S9">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -6586,8 +7148,14 @@
       <c r="Q10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>18</v>
+      </c>
+      <c r="S10">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -6630,8 +7198,14 @@
       <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -6674,8 +7248,14 @@
       <c r="Q12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -6718,8 +7298,14 @@
       <c r="Q13">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -6756,8 +7342,14 @@
       <c r="Q15">
         <v>1720</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>1578</v>
+      </c>
+      <c r="S15">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -6794,8 +7386,14 @@
       <c r="Q16">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <v>159</v>
+      </c>
+      <c r="S16">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -6863,8 +7461,16 @@
         <f t="shared" si="0"/>
         <v>1737</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <f t="shared" ref="R17:S17" si="1">SUM(R15, R16)</f>
+        <v>1737</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="1"/>
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -6873,201 +7479,225 @@
         <v>0</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" ref="C18:P18" si="1">C15/1737</f>
+        <f t="shared" ref="C18:P18" si="2">C15/1737</f>
         <v>0</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.94012665515256189</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.9654576856649395</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.98388025331030515</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99309153713298792</v>
       </c>
       <c r="K18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.94242947610823258</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.97063903281519859</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.98503166378814044</v>
       </c>
       <c r="N18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.99021301093839953</v>
       </c>
       <c r="O18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.86931491076568801</v>
       </c>
       <c r="P18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.86931491076568801</v>
       </c>
       <c r="Q18" s="2">
-        <f t="shared" ref="C18:Q18" si="2">Q15/1736</f>
+        <f t="shared" ref="Q18:S18" si="3">Q15/1736</f>
         <v>0.99078341013824889</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="2">
+        <f t="shared" si="3"/>
+        <v>0.90898617511520741</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="3"/>
+        <v>0.93605990783410142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
       <c r="B19" s="2">
-        <f t="shared" ref="B19:P20" si="3">B16/1737</f>
+        <f t="shared" ref="B19:P20" si="4">B16/1737</f>
         <v>0</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.9873344847438115E-2</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.4542314335060449E-2</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.6119746689694875E-2</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>6.9084628670120895E-3</v>
       </c>
       <c r="K19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.7570523891767415E-2</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.9360967184801381E-2</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.4968336211859529E-2</v>
       </c>
       <c r="N19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.7869890616004603E-3</v>
       </c>
       <c r="O19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.13068508923431202</v>
       </c>
       <c r="P19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.13068508923431202</v>
       </c>
       <c r="Q19" s="2">
-        <f t="shared" ref="B19:Q20" si="4">Q16/1736</f>
+        <f t="shared" ref="Q19:S20" si="5">Q16/1736</f>
         <v>9.7926267281105983E-3</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19" s="2">
+        <f t="shared" si="5"/>
+        <v>9.158986175115208E-2</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="5"/>
+        <v>6.4516129032258063E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="K20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="M20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="N20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="O20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="P20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
+        <v>1.0005760368663594</v>
+      </c>
+      <c r="R20" s="2">
+        <f t="shared" si="5"/>
+        <v>1.0005760368663594</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" si="5"/>
         <v>1.0005760368663594</v>
       </c>
     </row>

</xml_diff>